<commit_message>
added my name to the csv file
</commit_message>
<xml_diff>
--- a/peereval-Space-Z-Group.csv.xlsx
+++ b/peereval-Space-Z-Group.csv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erika\cs271\Space-Z-Group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johng\Desktop\cs371_Group_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A80DEA7B-E8FA-470A-B1E4-13C5A21F46B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C8ECDD-CD40-4BC1-A39D-1383E5283855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="840" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>ERIK ALVAREZ</t>
+  </si>
+  <si>
+    <t>Johnathon Garcia</t>
   </si>
 </sst>
 </file>
@@ -894,15 +897,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -913,7 +920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -924,48 +931,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>